<commit_message>
limpiando y borrando lo maximo
</commit_message>
<xml_diff>
--- a/ig/corecl/1.7.0/StructureDefinition-BundleCl.xlsx
+++ b/ig/corecl/1.7.0/StructureDefinition-BundleCl.xlsx
@@ -27,7 +27,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://hl7chile.cl/fhir/ig/corecl/StructureDefinition/BundleCl</t>
+    <t>https://hl7chile.cl/fhir/ig/CoreCL/StructureDefinition/BundleCl</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-12-07T13:24:22+00:00</t>
+    <t>2022-12-12T20:08:16-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1171,45 +1171,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.0078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.66015625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="21.21875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.77734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.26171875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.4453125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.1796875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="20.859375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="5.90234375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="142.140625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="140.08203125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.26953125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="168.19140625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="49.01171875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.59375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="34.98046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="11.0390625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="13.875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.71484375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.08984375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="163.2734375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="49.55078125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="14.98828125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="12.3046875" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="34.5859375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.87890625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="28.1484375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="24.98046875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="42.9765625" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="25.01171875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="22.67578125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="41.43359375" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="32.84375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>